<commit_message>
Edited docx file output
</commit_message>
<xml_diff>
--- a/histogram.xlsx
+++ b/histogram.xlsx
@@ -98,28 +98,28 @@
               <c:numCache>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>0.01</c:v>
+                  <c:v>0.02</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.01</c:v>
+                  <c:v>0.07</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.08</c:v>
+                  <c:v>0.21</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.24</c:v>
+                  <c:v>0.22</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.22</c:v>
+                  <c:v>0.28</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.23</c:v>
+                  <c:v>0.13</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.14</c:v>
+                  <c:v>0.05</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.08</c:v>
+                  <c:v>0.02</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -252,66 +252,66 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="n" s="0">
-        <v>84.94</v>
+        <v>73.69</v>
       </c>
       <c r="B1" t="n" s="0">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n" s="0">
-        <v>98.1</v>
+        <v>82.25</v>
       </c>
       <c r="B2" t="n" s="0">
-        <v>0.01</v>
+        <v>0.07</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n" s="0">
-        <v>111.28</v>
+        <v>90.79</v>
       </c>
       <c r="B3" t="n" s="0">
-        <v>0.08</v>
+        <v>0.21</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n" s="0">
-        <v>124.45</v>
+        <v>99.35</v>
       </c>
       <c r="B4" t="n" s="0">
-        <v>0.24</v>
+        <v>0.22</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n" s="0">
-        <v>137.62</v>
+        <v>107.89</v>
       </c>
       <c r="B5" t="n" s="0">
-        <v>0.22</v>
+        <v>0.28</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n" s="0">
-        <v>150.78</v>
+        <v>116.45</v>
       </c>
       <c r="B6" t="n" s="0">
-        <v>0.23</v>
+        <v>0.13</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n" s="0">
-        <v>163.96</v>
+        <v>124.99</v>
       </c>
       <c r="B7" t="n" s="0">
-        <v>0.14</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n" s="0">
-        <v>183.71</v>
+        <v>137.82</v>
       </c>
       <c r="B8" t="n" s="0">
-        <v>0.08</v>
+        <v>0.02</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Edit calculation of mediana and moda Edited docx file output (variation array and relative frequencies)
</commit_message>
<xml_diff>
--- a/histogram.xlsx
+++ b/histogram.xlsx
@@ -79,7 +79,7 @@
       <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
-        <c:varyColors val="true"/>
+        <c:varyColors val="false"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -110,10 +110,10 @@
                   <c:v>0.22</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.28</c:v>
+                  <c:v>0.29</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.13</c:v>
+                  <c:v>0.12</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0.05</c:v>
@@ -125,6 +125,7 @@
             </c:numRef>
           </c:val>
         </c:ser>
+        <c:gapWidth val="2"/>
         <c:axId val="0"/>
         <c:axId val="1"/>
       </c:barChart>
@@ -252,7 +253,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="n" s="0">
-        <v>73.69</v>
+        <v>73.7</v>
       </c>
       <c r="B1" t="n" s="0">
         <v>0.02</v>
@@ -260,7 +261,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n" s="0">
-        <v>82.25</v>
+        <v>82.26</v>
       </c>
       <c r="B2" t="n" s="0">
         <v>0.07</v>
@@ -268,7 +269,7 @@
     </row>
     <row r="3">
       <c r="A3" t="n" s="0">
-        <v>90.79</v>
+        <v>90.82</v>
       </c>
       <c r="B3" t="n" s="0">
         <v>0.21</v>
@@ -276,7 +277,7 @@
     </row>
     <row r="4">
       <c r="A4" t="n" s="0">
-        <v>99.35</v>
+        <v>99.38</v>
       </c>
       <c r="B4" t="n" s="0">
         <v>0.22</v>
@@ -284,23 +285,23 @@
     </row>
     <row r="5">
       <c r="A5" t="n" s="0">
-        <v>107.89</v>
+        <v>107.94</v>
       </c>
       <c r="B5" t="n" s="0">
-        <v>0.28</v>
+        <v>0.29</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n" s="0">
-        <v>116.45</v>
+        <v>116.5</v>
       </c>
       <c r="B6" t="n" s="0">
-        <v>0.13</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n" s="0">
-        <v>124.99</v>
+        <v>125.06</v>
       </c>
       <c r="B7" t="n" s="0">
         <v>0.05</v>
@@ -308,7 +309,7 @@
     </row>
     <row r="8">
       <c r="A8" t="n" s="0">
-        <v>137.82</v>
+        <v>133.62</v>
       </c>
       <c r="B8" t="n" s="0">
         <v>0.02</v>

</xml_diff>